<commit_message>
Added a protocol, some description and changed the result list
</commit_message>
<xml_diff>
--- a/Practical8/Autophagosome.xlsx
+++ b/Practical8/Autophagosome.xlsx
@@ -1163,7 +1163,7 @@
         <v>105</v>
       </c>
       <c r="D33">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1177,7 +1177,7 @@
         <v>106</v>
       </c>
       <c r="D34">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1191,7 +1191,7 @@
         <v>107</v>
       </c>
       <c r="D35">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1205,7 +1205,7 @@
         <v>108</v>
       </c>
       <c r="D36">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>